<commit_message>
Minor edits to the color sheet
</commit_message>
<xml_diff>
--- a/Color Ranges.xlsx
+++ b/Color Ranges.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Syncs\Repos\WhatColor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1020CDCA-EBA4-4EAB-8A3A-C442F364B197}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E030EFC4-5EEB-4D79-9131-095144DC790F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="table-1" sheetId="1" r:id="rId1"/>
+    <sheet name="What Color" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
@@ -14927,7 +14927,7 @@
   <dimension ref="A1:K975"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Attempt 1 at adding all color ranges md sheet
</commit_message>
<xml_diff>
--- a/Color Ranges.xlsx
+++ b/Color Ranges.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Syncs\Repos\WhatColor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0856FAB3-AFF1-44D0-9AD5-4EC8A4B70BF5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D36762DE-C0A7-436F-A6EE-859F8BCCF0F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15211,8 +15211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K996"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A955" workbookViewId="0">
-      <selection activeCell="N974" sqref="N974"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>